<commit_message>
feature: support hyper link
</commit_message>
<xml_diff>
--- a/demo/template.xlsx
+++ b/demo/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16100" tabRatio="500"/>
+    <workbookView windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="2" r:id="rId1"/>
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
   <si>
     <t>Hello {{name}}</t>
   </si>
   <si>
     <t>Here is a list of your items</t>
-  </si>
-  <si>
-    <t>可以</t>
   </si>
   <si>
     <t>{{nameHeader}}</t>
@@ -45,16 +42,25 @@
   <si>
     <t>{{end}}</t>
   </si>
+  <si>
+    <t>{{url}}</t>
+  </si>
+  <si>
+    <t>{{file}}</t>
+  </si>
+  <si>
+    <t>https://github.com/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -80,6 +86,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -87,6 +101,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,6 +118,81 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,62 +207,16 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,51 +229,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -245,31 +251,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,25 +395,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,109 +425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,20 +500,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,6 +530,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -542,6 +554,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -556,190 +597,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -766,6 +772,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,10 +1093,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.8" outlineLevelCol="4"/>
@@ -1114,21 +1122,19 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" ht="15.95" spans="1:5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="15.2" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -1138,28 +1144,46 @@
     <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A10" r:id="rId1" display="{{url}}"/>
+    <hyperlink ref="B10" r:id="rId2" display="{{file}}"/>
+    <hyperlink ref="A11" r:id="rId1" display="https://github.com/"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>